<commit_message>
para agregar codigo de barras
</commit_message>
<xml_diff>
--- a/reportes/10.10.2.25.xlsx
+++ b/reportes/10.10.2.25.xlsx
@@ -31,10 +31,10 @@
     <t>No. Expediente Clínico</t>
   </si>
   <si>
-    <t>VELA  RODRIGUEZ  MARVIN  FRANCISCO</t>
-  </si>
-  <si>
-    <t>/201769603</t>
+    <t>MONTERROSO  LÓPEZ  CRISTIAN  JOSUÉ</t>
+  </si>
+  <si>
+    <t>/201773491</t>
   </si>
   <si>
     <t>Fecha de Nacimiento ( Dia Mes Año)</t>
@@ -49,13 +49,13 @@
     <t>Sexo M  (   )   F  (    )</t>
   </si>
   <si>
-    <t>1984-10-08</t>
-  </si>
-  <si>
-    <t>33</t>
-  </si>
-  <si>
-    <t>EL PROGRESO GUSTATOYA</t>
+    <t>1993-02-23</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>CHINAUTLA</t>
   </si>
   <si>
     <t>MASCULINO</t>
@@ -76,13 +76,13 @@
     <t>SOLTERO</t>
   </si>
   <si>
-    <t>COMERCIANTE</t>
-  </si>
-  <si>
-    <t>GUATEMALTECA</t>
-  </si>
-  <si>
-    <t>NO PRESENTO</t>
+    <t>VARIOS</t>
+  </si>
+  <si>
+    <t>GUATEMALTECO</t>
+  </si>
+  <si>
+    <t>2201016710106</t>
   </si>
   <si>
     <t>En caso de emergencia notificar a:</t>
@@ -97,28 +97,28 @@
     <t>Teléfono</t>
   </si>
   <si>
-    <t>SOLO</t>
-  </si>
-  <si>
-    <t>NINGUNO</t>
-  </si>
-  <si>
-    <t>BARRIO LA JOYA EL PROGRESO</t>
-  </si>
-  <si>
-    <t>NO TIENE</t>
+    <t>ANDREA MORENO</t>
+  </si>
+  <si>
+    <t>ENCARGADA</t>
+  </si>
+  <si>
+    <t>34 AV 12-16 Z. 5 EL EDEN</t>
+  </si>
+  <si>
+    <t>49803299</t>
   </si>
   <si>
     <t>Fecha de la asistencia Médica</t>
   </si>
   <si>
-    <t>Hora: 15:33:36</t>
+    <t>Hora: 15:45:35</t>
   </si>
   <si>
     <t>Area de urgencia: MEDICINA</t>
   </si>
   <si>
-    <t>10/11/2017</t>
+    <t>20/11/2017</t>
   </si>
   <si>
     <t>MEDICINA</t>

</xml_diff>